<commit_message>
Updated exerimental parameters. Added calculation for approximate session duration
</commit_message>
<xml_diff>
--- a/vr_screen_params.xlsx
+++ b/vr_screen_params.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
   <si>
     <t>speed</t>
   </si>
@@ -32,9 +32,6 @@
     <t>acceleration</t>
   </si>
   <si>
-    <t>contrast</t>
-  </si>
-  <si>
     <t>object</t>
   </si>
   <si>
@@ -44,51 +41,24 @@
     <t>notes</t>
   </si>
   <si>
-    <t>[0.25, 0.5, 1]</t>
-  </si>
-  <si>
     <t>scale</t>
   </si>
   <si>
-    <t>[0.5]</t>
-  </si>
-  <si>
     <t>[0.15]</t>
   </si>
   <si>
     <t>[0]</t>
   </si>
   <si>
-    <t>[1]</t>
-  </si>
-  <si>
-    <t>[0.75]</t>
-  </si>
-  <si>
     <t>repetitions</t>
   </si>
   <si>
-    <t>[0, 1, 2]</t>
-  </si>
-  <si>
     <t>sortby</t>
   </si>
   <si>
-    <t>['contrast']</t>
-  </si>
-  <si>
     <t>isi</t>
   </si>
   <si>
-    <t>[0.1, 0.15]</t>
-  </si>
-  <si>
-    <t>[0.05]</t>
-  </si>
-  <si>
-    <t>[0.25, 0]</t>
-  </si>
-  <si>
     <t>[0.2]</t>
   </si>
   <si>
@@ -98,7 +68,40 @@
     <t>test</t>
   </si>
   <si>
-    <t>[1.0, 0.75, 0.5, 0.25]</t>
+    <t>color_screen</t>
+  </si>
+  <si>
+    <t>color_target</t>
+  </si>
+  <si>
+    <t>[(1, 1, 1, 1)]</t>
+  </si>
+  <si>
+    <t>[(0, 0, 0, 1)]</t>
+  </si>
+  <si>
+    <t>[(1, 1, 1, 1), (0.5, 0.5, 0.5, 1)]</t>
+  </si>
+  <si>
+    <t>[(0.05, 0, 0.05)]</t>
+  </si>
+  <si>
+    <t>first experiment</t>
+  </si>
+  <si>
+    <t>[0.02, 0.15, 0.25, 0.5, 0.75]</t>
+  </si>
+  <si>
+    <t>[10]</t>
+  </si>
+  <si>
+    <t>[(0.01, 0, 0.01), (0.02, 0, 0.02), (0.04, 0, 0.04), (0.06, 0, 0.06),(0.08, 0, 0.08)]</t>
+  </si>
+  <si>
+    <t>[(0, 0, 0, 1), (0.25, 0.25, 0.25, 1)]</t>
+  </si>
+  <si>
+    <t>[0.02, 0.07, 0.15, 0.3, 0.5]</t>
   </si>
 </sst>
 </file>
@@ -141,9 +144,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,137 +428,153 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.42578125" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" customWidth="1"/>
-    <col min="9" max="9" width="8" customWidth="1"/>
-    <col min="10" max="10" width="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="66.7109375" customWidth="1"/>
+    <col min="3" max="3" width="26.28515625" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" customWidth="1"/>
+    <col min="5" max="5" width="35.140625" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" customWidth="1"/>
+    <col min="10" max="10" width="8" customWidth="1"/>
+    <col min="11" max="11" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="I2">
+        <v>5</v>
+      </c>
+      <c r="J2">
+        <v>3</v>
+      </c>
+      <c r="K2" t="s">
         <v>13</v>
       </c>
-      <c r="I1" t="s">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
         <v>17</v>
       </c>
-      <c r="J1" t="s">
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3">
         <v>5</v>
       </c>
+      <c r="J3">
+        <v>3</v>
+      </c>
+      <c r="K3" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" t="s">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
         <v>16</v>
       </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2">
+      <c r="D4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4">
+        <v>5</v>
+      </c>
+      <c r="J4">
         <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4">
-        <v>3</v>
-      </c>
-      <c r="I4">
-        <v>3</v>
-      </c>
-      <c r="J4" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated exerimental parameters and modified start delay times
</commit_message>
<xml_diff>
--- a/vr_screen_params.xlsx
+++ b/vr_screen_params.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
   <si>
     <t>speed</t>
   </si>
@@ -32,9 +32,6 @@
     <t>acceleration</t>
   </si>
   <si>
-    <t>contrast</t>
-  </si>
-  <si>
     <t>object</t>
   </si>
   <si>
@@ -44,51 +41,24 @@
     <t>notes</t>
   </si>
   <si>
-    <t>[0.25, 0.5, 1]</t>
-  </si>
-  <si>
     <t>scale</t>
   </si>
   <si>
-    <t>[0.5]</t>
-  </si>
-  <si>
     <t>[0.15]</t>
   </si>
   <si>
     <t>[0]</t>
   </si>
   <si>
-    <t>[1]</t>
-  </si>
-  <si>
-    <t>[0.75]</t>
-  </si>
-  <si>
     <t>repetitions</t>
   </si>
   <si>
-    <t>[0, 1, 2]</t>
-  </si>
-  <si>
     <t>sortby</t>
   </si>
   <si>
-    <t>['contrast']</t>
-  </si>
-  <si>
     <t>isi</t>
   </si>
   <si>
-    <t>[0.1, 0.15]</t>
-  </si>
-  <si>
-    <t>[0.05]</t>
-  </si>
-  <si>
-    <t>[0.25, 0]</t>
-  </si>
-  <si>
     <t>[0.2]</t>
   </si>
   <si>
@@ -98,7 +68,40 @@
     <t>test</t>
   </si>
   <si>
-    <t>[1.0, 0.75, 0.5, 0.25]</t>
+    <t>color_screen</t>
+  </si>
+  <si>
+    <t>color_target</t>
+  </si>
+  <si>
+    <t>[(1, 1, 1, 1)]</t>
+  </si>
+  <si>
+    <t>[(0, 0, 0, 1)]</t>
+  </si>
+  <si>
+    <t>[(1, 1, 1, 1), (0.5, 0.5, 0.5, 1)]</t>
+  </si>
+  <si>
+    <t>[(0.05, 0, 0.05)]</t>
+  </si>
+  <si>
+    <t>first experiment</t>
+  </si>
+  <si>
+    <t>[0.02, 0.15, 0.25, 0.5, 0.75]</t>
+  </si>
+  <si>
+    <t>[10]</t>
+  </si>
+  <si>
+    <t>[(0.01, 0, 0.01), (0.02, 0, 0.02), (0.04, 0, 0.04), (0.06, 0, 0.06),(0.08, 0, 0.08)]</t>
+  </si>
+  <si>
+    <t>[0.02, 0.05, 0.07, 0.10, 0.15, 0.25, 0.5]</t>
+  </si>
+  <si>
+    <t>[(0, 0, 0, 1), (0.25, 0.25, 0.25, 1)]</t>
   </si>
 </sst>
 </file>
@@ -141,9 +144,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,137 +428,153 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.42578125" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" customWidth="1"/>
-    <col min="9" max="9" width="8" customWidth="1"/>
-    <col min="10" max="10" width="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="66.7109375" customWidth="1"/>
+    <col min="3" max="3" width="26.28515625" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" customWidth="1"/>
+    <col min="5" max="5" width="35.140625" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" customWidth="1"/>
+    <col min="10" max="10" width="8" customWidth="1"/>
+    <col min="11" max="11" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="B2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
         <v>17</v>
       </c>
-      <c r="J1" t="s">
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2">
         <v>5</v>
       </c>
+      <c r="J2">
+        <v>3</v>
+      </c>
+      <c r="K2" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" t="s">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
         <v>16</v>
       </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2">
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3">
+        <v>5</v>
+      </c>
+      <c r="J3">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>12</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>22</v>
       </c>
       <c r="B4" t="s">
         <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4">
+        <v>6</v>
+      </c>
+      <c r="G4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4">
+        <v>5</v>
+      </c>
+      <c r="J4">
         <v>3</v>
       </c>
-      <c r="I4">
-        <v>3</v>
-      </c>
-      <c r="J4" t="s">
-        <v>23</v>
+      <c r="K4" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes to distance calculation for VRScreenTrialStructure
</commit_message>
<xml_diff>
--- a/vr_screen_params.xlsx
+++ b/vr_screen_params.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="42">
   <si>
     <t>speed</t>
   </si>
@@ -102,6 +102,54 @@
   </si>
   <si>
     <t>[0.02, 0.07, 0.15, 0.3, 0.5]</t>
+  </si>
+  <si>
+    <t>first 3D</t>
+  </si>
+  <si>
+    <t>[3]</t>
+  </si>
+  <si>
+    <t>[(0.01, 0.01, 0.01), (0.02, 0.02, 0.02), (0.04, 0.04, 0.04), (0.06, 0.06, 0.06),(0.08, 0.08, 0.08)]</t>
+  </si>
+  <si>
+    <t>redo 2D with fixes</t>
+  </si>
+  <si>
+    <t>redo 3D with fixes</t>
+  </si>
+  <si>
+    <t>[0.02, 0.07, 0.15, 0.3]</t>
+  </si>
+  <si>
+    <t>[0, 3]</t>
+  </si>
+  <si>
+    <t>[(0, 0.01, 0.01), (0, 0.02, 0.02), (0, 0.04, 0.04), (0, 0.08, 0.08)]</t>
+  </si>
+  <si>
+    <t>[(0, 0, 0, 1), (0.25, 0.25, 0.25, 1),  (0.5, 0.5, 0.5, 1)]</t>
+  </si>
+  <si>
+    <t>[(0.01, 0.01, 0.01), (0.02, 0.02, 0.02), (0.04, 0.04, 0.04), (0.08, 0.08, 0.08)]</t>
+  </si>
+  <si>
+    <t>new combined stim, first exp</t>
+  </si>
+  <si>
+    <t>[0.02, 0.07, 0.15]</t>
+  </si>
+  <si>
+    <t>[(0.01, 0.01, 0.01), (0.04, 0.04, 0.04), (0.08, 0.08, 0.08)]</t>
+  </si>
+  <si>
+    <t>[(0, 0, 0, 1), (0.25, 0.25, 0.25, 1), (1, 1, 1, 1)]</t>
+  </si>
+  <si>
+    <t>[0.02, 0.15, 0.30]</t>
+  </si>
+  <si>
+    <t>[(0.02, 0.02, 0.02), (0.06, 0.06, 0.06),(0.08, 0.08, 0.08)]</t>
   </si>
 </sst>
 </file>
@@ -428,18 +476,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="66.7109375" customWidth="1"/>
+    <col min="2" max="2" width="77.140625" customWidth="1"/>
     <col min="3" max="3" width="26.28515625" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" customWidth="1"/>
+    <col min="4" max="4" width="35.42578125" customWidth="1"/>
     <col min="5" max="5" width="35.140625" customWidth="1"/>
     <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
@@ -577,6 +625,221 @@
         <v>3</v>
       </c>
     </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5">
+        <v>5</v>
+      </c>
+      <c r="J5">
+        <v>3</v>
+      </c>
+      <c r="K5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I6">
+        <v>5</v>
+      </c>
+      <c r="J6">
+        <v>3</v>
+      </c>
+      <c r="K6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7">
+        <v>3</v>
+      </c>
+      <c r="J7">
+        <v>3</v>
+      </c>
+      <c r="K7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I8">
+        <v>3</v>
+      </c>
+      <c r="J8">
+        <v>2</v>
+      </c>
+      <c r="K8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" t="s">
+        <v>7</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I11">
+        <v>2</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Moved VSCreenTrialStrcuture class to its own file
</commit_message>
<xml_diff>
--- a/vr_screen_params.xlsx
+++ b/vr_screen_params.xlsx
@@ -149,7 +149,7 @@
     <t>[0.02, 0.15, 0.30]</t>
   </si>
   <si>
-    <t>[(0.02, 0.02, 0.02), (0.06, 0.06, 0.06),(0.08, 0.08, 0.08)]</t>
+    <t>[(0.02, 0.02, 0.02), (0.06, 0.06, 0.06), (0.08, 0.08, 0.08)]</t>
   </si>
 </sst>
 </file>
@@ -479,7 +479,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>